<commit_message>
ajustes sanity semilla 6
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla6\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F07928-93B4-448E-AF16-E4A194849F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B1EF2-3B4B-4524-9F64-4C05A2EAA1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 6" sheetId="4" r:id="rId1"/>
-    <sheet name="Semilla 3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>MSIDN</t>
   </si>
@@ -58,9 +57,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>DEV11G</t>
-  </si>
-  <si>
     <t>ACTIVATOR</t>
   </si>
   <si>
@@ -112,42 +108,6 @@
     <t>C:\Program Files (x86)\Winwap Technologies\WinWAP for Windows 4.2\WinWAP4.exe</t>
   </si>
   <si>
-    <t>http://10.69.60.106:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
-    <t>http://10.69.60.106:8180/tigo-pos-web/index.jsp</t>
-  </si>
-  <si>
-    <t>10.69.60.103</t>
-  </si>
-  <si>
-    <t>10.69.60.102</t>
-  </si>
-  <si>
-    <t>10.65.32.76</t>
-  </si>
-  <si>
-    <t>SIEBEL02</t>
-  </si>
-  <si>
-    <t>732111324707274</t>
-  </si>
-  <si>
-    <t>3043208091</t>
-  </si>
-  <si>
-    <t>3043209773</t>
-  </si>
-  <si>
-    <t>732111324707275</t>
-  </si>
-  <si>
-    <t>732111324707276</t>
-  </si>
-  <si>
-    <t>732111324707277</t>
-  </si>
-  <si>
     <t>3045981684</t>
   </si>
   <si>
@@ -223,12 +183,6 @@
     <t>SIEBEL03</t>
   </si>
   <si>
-    <t>10.69.60.105</t>
-  </si>
-  <si>
-    <t>http://10.69.60.107:8280/portal/login?initialURI=%2Fportal%2FCRMPortal%2FVenta</t>
-  </si>
-  <si>
     <t>http://10.69.60.75:8180/tigo-pos-web/index.jsp</t>
   </si>
   <si>
@@ -238,34 +192,55 @@
     <t>http://10.69.60.75:8180/tigo-pos-web/wap/windex.wml</t>
   </si>
   <si>
-    <t>585087750</t>
-  </si>
-  <si>
-    <t>126601516</t>
-  </si>
-  <si>
-    <t>256424866</t>
-  </si>
-  <si>
-    <t>681590982</t>
-  </si>
-  <si>
-    <t>884243417</t>
-  </si>
-  <si>
-    <t>3045981670</t>
-  </si>
-  <si>
     <t>10.69.60.74</t>
   </si>
   <si>
-    <t>3043209863</t>
-  </si>
-  <si>
-    <t>3043209819</t>
-  </si>
-  <si>
-    <t>3043209868</t>
+    <t>657040817</t>
+  </si>
+  <si>
+    <t>845393501</t>
+  </si>
+  <si>
+    <t>645988527</t>
+  </si>
+  <si>
+    <t>903350907</t>
+  </si>
+  <si>
+    <t>417771447</t>
+  </si>
+  <si>
+    <t>3046010569</t>
+  </si>
+  <si>
+    <t>732111193280551</t>
+  </si>
+  <si>
+    <t>3052754289</t>
+  </si>
+  <si>
+    <t>732111324709674</t>
+  </si>
+  <si>
+    <t>3052754293</t>
+  </si>
+  <si>
+    <t>732111324709675</t>
+  </si>
+  <si>
+    <t>3052754321</t>
+  </si>
+  <si>
+    <t>732111324709676</t>
+  </si>
+  <si>
+    <t>3046008587</t>
+  </si>
+  <si>
+    <t>732111193280535</t>
+  </si>
+  <si>
+    <t>1011218853</t>
   </si>
 </sst>
 </file>
@@ -346,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -369,6 +344,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -684,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D188C588-523E-4AEF-A066-FA5DCECDB773}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -722,39 +700,39 @@
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="I2" s="7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1">
@@ -762,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -773,205 +751,219 @@
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -986,310 +978,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1">
-      <c r="A5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1">
-      <c r="A6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1">
-      <c r="A7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="I2" r:id="rId6" xr:uid="{F95E11DB-0174-40E5-880B-10A9CAE9721D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Se crean nuevos casos para cesion de contrato nit a nit
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla6\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\-SanitySemilla6\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B1EF2-3B4B-4524-9F64-4C05A2EAA1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE190472-72F7-4ABB-9974-BCBF76AC4119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 6" sheetId="4" r:id="rId1"/>
+    <sheet name="Semilla 3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="80">
   <si>
     <t>MSIDN</t>
   </si>
@@ -57,6 +58,9 @@
     <t>password</t>
   </si>
   <si>
+    <t>DEV11G</t>
+  </si>
+  <si>
     <t>ACTIVATOR</t>
   </si>
   <si>
@@ -108,7 +112,22 @@
     <t>C:\Program Files (x86)\Winwap Technologies\WinWAP for Windows 4.2\WinWAP4.exe</t>
   </si>
   <si>
-    <t>3045981684</t>
+    <t>http://10.69.60.106:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>http://10.69.60.106:8180/tigo-pos-web/index.jsp</t>
+  </si>
+  <si>
+    <t>10.69.60.103</t>
+  </si>
+  <si>
+    <t>10.69.60.102</t>
+  </si>
+  <si>
+    <t>10.65.32.76</t>
+  </si>
+  <si>
+    <t>SIEBEL02</t>
   </si>
   <si>
     <t>732111193278813</t>
@@ -156,9 +175,6 @@
     <t>732111193278730</t>
   </si>
   <si>
-    <t>3045984642</t>
-  </si>
-  <si>
     <t>host ssh</t>
   </si>
   <si>
@@ -183,6 +199,12 @@
     <t>SIEBEL03</t>
   </si>
   <si>
+    <t>10.69.60.105</t>
+  </si>
+  <si>
+    <t>http://10.69.60.107:8280/portal/login?initialURI=%2Fportal%2FCRMPortal%2FVenta</t>
+  </si>
+  <si>
     <t>http://10.69.60.75:8180/tigo-pos-web/index.jsp</t>
   </si>
   <si>
@@ -192,62 +214,65 @@
     <t>http://10.69.60.75:8180/tigo-pos-web/wap/windex.wml</t>
   </si>
   <si>
+    <t>585087750</t>
+  </si>
+  <si>
+    <t>126601516</t>
+  </si>
+  <si>
+    <t>256424866</t>
+  </si>
+  <si>
+    <t>681590982</t>
+  </si>
+  <si>
+    <t>884243417</t>
+  </si>
+  <si>
     <t>10.69.60.74</t>
   </si>
   <si>
-    <t>657040817</t>
-  </si>
-  <si>
-    <t>845393501</t>
-  </si>
-  <si>
-    <t>645988527</t>
-  </si>
-  <si>
-    <t>903350907</t>
-  </si>
-  <si>
-    <t>417771447</t>
-  </si>
-  <si>
     <t>3046010569</t>
   </si>
   <si>
+    <t>3052754289</t>
+  </si>
+  <si>
+    <t>3052754293</t>
+  </si>
+  <si>
+    <t>3052754321</t>
+  </si>
+  <si>
+    <t>3046008587</t>
+  </si>
+  <si>
     <t>732111193280551</t>
   </si>
   <si>
-    <t>3052754289</t>
-  </si>
-  <si>
     <t>732111324709674</t>
   </si>
   <si>
-    <t>3052754293</t>
-  </si>
-  <si>
     <t>732111324709675</t>
   </si>
   <si>
-    <t>3052754321</t>
-  </si>
-  <si>
     <t>732111324709676</t>
   </si>
   <si>
-    <t>3046008587</t>
-  </si>
-  <si>
     <t>732111193280535</t>
   </si>
   <si>
-    <t>1011218853</t>
+    <t>3045984556</t>
+  </si>
+  <si>
+    <t>3052749177</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +324,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -344,9 +377,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -664,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D188C588-523E-4AEF-A066-FA5DCECDB773}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -700,39 +731,39 @@
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1">
@@ -740,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -751,219 +782,219 @@
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="10" t="s">
         <v>62</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>64</v>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>66</v>
+      <c r="C12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -978,4 +1009,330 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" s="10"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I2" r:id="rId6" xr:uid="{F95E11DB-0174-40E5-880B-10A9CAE9721D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ajustes sanity semilla 6 en clases de portabilidad prepago y postpago
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla6\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B1EF2-3B4B-4524-9F64-4C05A2EAA1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348E1D0E-A581-4A9C-8561-83E6482D4609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31965" yWindow="5145" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 6" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
   <si>
     <t>MSIDN</t>
   </si>
@@ -132,9 +132,6 @@
     <t>client</t>
   </si>
   <si>
-    <t>1061520830</t>
-  </si>
-  <si>
     <t>111295346</t>
   </si>
   <si>
@@ -150,15 +147,9 @@
     <t>URL Portabilidad SoapUI</t>
   </si>
   <si>
-    <t>http://10.69.60.76:8080/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl</t>
-  </si>
-  <si>
     <t>732111193278730</t>
   </si>
   <si>
-    <t>3045984642</t>
-  </si>
-  <si>
     <t>host ssh</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
     <t>903350907</t>
   </si>
   <si>
-    <t>417771447</t>
-  </si>
-  <si>
     <t>3046010569</t>
   </si>
   <si>
@@ -241,6 +229,15 @@
   </si>
   <si>
     <t>1011218853</t>
+  </si>
+  <si>
+    <t>662496115</t>
+  </si>
+  <si>
+    <t>3046008600</t>
+  </si>
+  <si>
+    <t>http://10.69.60.74:8080/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl</t>
   </si>
 </sst>
 </file>
@@ -664,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D188C588-523E-4AEF-A066-FA5DCECDB773}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -703,18 +700,18 @@
         <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
@@ -732,7 +729,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1">
@@ -751,10 +748,10 @@
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
@@ -763,18 +760,18 @@
         <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
@@ -786,18 +783,18 @@
         <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
@@ -814,7 +811,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>16</v>
@@ -849,7 +846,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
@@ -857,13 +854,13 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>27</v>
@@ -875,10 +872,10 @@
         <v>32</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
@@ -886,28 +883,28 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1">
@@ -915,13 +912,13 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1">
@@ -929,13 +926,13 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1">
@@ -943,13 +940,13 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -957,13 +954,13 @@
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>